<commit_message>
add file list library
</commit_message>
<xml_diff>
--- a/DATA_BRAZIL/GIAOHOI.xlsx
+++ b/DATA_BRAZIL/GIAOHOI.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WBPC.VN\PycharmProjects\scrapDataWeb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -3646,8 +3651,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3697,6 +3702,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3743,7 +3756,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3775,9 +3788,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3809,6 +3823,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3984,14 +3999,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="5" width="49" customWidth="1"/>
+    <col min="6" max="6" width="68.7109375" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4020,7 +4045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4049,7 +4074,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -4078,7 +4103,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4107,7 +4132,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -4136,7 +4161,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -4165,7 +4190,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -4194,7 +4219,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -4223,7 +4248,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -4252,7 +4277,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4281,7 +4306,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4310,7 +4335,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -4339,7 +4364,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -4368,7 +4393,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -4397,7 +4422,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -4426,7 +4451,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -4455,7 +4480,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -4484,7 +4509,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -4513,7 +4538,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -4542,7 +4567,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -4568,7 +4593,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -4597,7 +4622,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -4626,7 +4651,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -4655,7 +4680,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -4684,7 +4709,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -4713,7 +4738,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -4742,7 +4767,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -4771,7 +4796,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -4800,7 +4825,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -4829,7 +4854,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -4858,7 +4883,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -4887,7 +4912,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -4916,7 +4941,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -4945,7 +4970,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -4974,7 +4999,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -5003,7 +5028,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -5032,7 +5057,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -5061,7 +5086,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -5090,7 +5115,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -5119,7 +5144,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -5148,7 +5173,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -5177,7 +5202,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -5206,7 +5231,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -5235,7 +5260,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -5264,7 +5289,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -5293,7 +5318,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -5322,7 +5347,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -5351,7 +5376,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -5380,7 +5405,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -5409,7 +5434,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -5438,7 +5463,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -5467,7 +5492,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -5496,7 +5521,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -5525,7 +5550,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -5554,7 +5579,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -5583,7 +5608,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>9</v>
       </c>
@@ -5612,7 +5637,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -5641,7 +5666,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -5670,7 +5695,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -5699,7 +5724,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -5728,7 +5753,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -5757,7 +5782,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>9</v>
       </c>
@@ -5786,7 +5811,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -5815,7 +5840,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -5841,7 +5866,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>9</v>
       </c>
@@ -5867,7 +5892,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>9</v>
       </c>
@@ -5896,7 +5921,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -5925,7 +5950,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>9</v>
       </c>
@@ -5954,7 +5979,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>9</v>
       </c>
@@ -5983,7 +6008,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>9</v>
       </c>
@@ -6009,7 +6034,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>9</v>
       </c>
@@ -6038,7 +6063,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -6067,7 +6092,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>9</v>
       </c>
@@ -6096,7 +6121,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>9</v>
       </c>
@@ -6125,7 +6150,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -6154,7 +6179,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -6180,7 +6205,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>9</v>
       </c>
@@ -6209,7 +6234,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -6238,7 +6263,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -6267,7 +6292,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>9</v>
       </c>
@@ -6296,7 +6321,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -6325,7 +6350,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>9</v>
       </c>
@@ -6354,7 +6379,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -6383,7 +6408,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>9</v>
       </c>
@@ -6412,7 +6437,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>9</v>
       </c>
@@ -6441,7 +6466,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>9</v>
       </c>
@@ -6467,7 +6492,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -6496,7 +6521,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>9</v>
       </c>
@@ -6525,7 +6550,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>9</v>
       </c>
@@ -6554,7 +6579,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>9</v>
       </c>
@@ -6580,7 +6605,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>9</v>
       </c>
@@ -6609,7 +6634,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>9</v>
       </c>
@@ -6638,7 +6663,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -6667,7 +6692,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -6693,7 +6718,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -6722,7 +6747,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>9</v>
       </c>
@@ -6751,7 +6776,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>9</v>
       </c>
@@ -6780,7 +6805,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -6809,7 +6834,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -6838,7 +6863,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -6864,7 +6889,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -6893,7 +6918,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -6922,7 +6947,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -6951,7 +6976,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -6977,7 +7002,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>9</v>
       </c>
@@ -7006,7 +7031,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>9</v>
       </c>
@@ -7035,7 +7060,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>9</v>
       </c>
@@ -7064,7 +7089,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -7093,7 +7118,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -7122,7 +7147,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -7148,7 +7173,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -7177,7 +7202,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>9</v>
       </c>
@@ -7206,7 +7231,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>9</v>
       </c>
@@ -7235,7 +7260,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>9</v>
       </c>
@@ -7261,7 +7286,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>9</v>
       </c>
@@ -7290,7 +7315,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -7319,7 +7344,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -7348,7 +7373,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -7377,7 +7402,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -7403,7 +7428,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -7432,7 +7457,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>9</v>
       </c>
@@ -7461,7 +7486,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>9</v>
       </c>
@@ -7487,7 +7512,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>9</v>
       </c>
@@ -7516,7 +7541,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -7545,7 +7570,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -7574,7 +7599,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -7603,7 +7628,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>9</v>
       </c>
@@ -7632,7 +7657,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>9</v>
       </c>
@@ -7661,7 +7686,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -7690,7 +7715,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>9</v>
       </c>
@@ -7719,7 +7744,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>9</v>
       </c>
@@ -7748,7 +7773,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>9</v>
       </c>
@@ -7774,7 +7799,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>9</v>
       </c>
@@ -7803,7 +7828,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>9</v>
       </c>
@@ -7832,7 +7857,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -7861,7 +7886,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -7887,7 +7912,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>9</v>
       </c>
@@ -7916,7 +7941,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>9</v>
       </c>
@@ -7945,7 +7970,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -7974,7 +7999,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -8003,7 +8028,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -8032,7 +8057,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>9</v>
       </c>
@@ -8061,7 +8086,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -8090,7 +8115,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -8119,7 +8144,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>9</v>
       </c>
@@ -8145,7 +8170,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>9</v>
       </c>
@@ -8174,7 +8199,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -8203,7 +8228,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>9</v>
       </c>
@@ -8232,7 +8257,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -8261,7 +8286,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>9</v>
       </c>
@@ -8290,7 +8315,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>9</v>
       </c>
@@ -8319,7 +8344,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>9</v>
       </c>
@@ -8345,7 +8370,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>9</v>
       </c>
@@ -8374,7 +8399,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>9</v>
       </c>
@@ -8403,7 +8428,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>9</v>
       </c>
@@ -8432,7 +8457,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>9</v>
       </c>
@@ -8461,7 +8486,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -8490,7 +8515,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>9</v>
       </c>
@@ -8519,7 +8544,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>9</v>
       </c>
@@ -8548,7 +8573,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>9</v>
       </c>
@@ -8577,7 +8602,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>9</v>
       </c>
@@ -8603,7 +8628,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>9</v>
       </c>
@@ -8629,7 +8654,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>9</v>
       </c>
@@ -8658,7 +8683,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>9</v>
       </c>
@@ -8684,7 +8709,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>9</v>
       </c>
@@ -8713,7 +8738,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>9</v>
       </c>
@@ -8742,7 +8767,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>9</v>
       </c>
@@ -8771,7 +8796,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>9</v>
       </c>
@@ -8797,7 +8822,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>9</v>
       </c>
@@ -8826,7 +8851,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>9</v>
       </c>
@@ -8855,7 +8880,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>9</v>
       </c>
@@ -8884,7 +8909,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>9</v>
       </c>
@@ -8913,7 +8938,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>9</v>
       </c>
@@ -8942,7 +8967,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>9</v>
       </c>
@@ -8971,7 +8996,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>9</v>
       </c>
@@ -9000,7 +9025,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>9</v>
       </c>
@@ -9029,7 +9054,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>9</v>
       </c>
@@ -9055,7 +9080,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>9</v>
       </c>
@@ -9084,7 +9109,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>9</v>
       </c>
@@ -9110,7 +9135,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>9</v>
       </c>
@@ -9139,7 +9164,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>9</v>
       </c>
@@ -9168,7 +9193,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>9</v>
       </c>
@@ -9197,7 +9222,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>9</v>
       </c>
@@ -9226,7 +9251,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>9</v>
       </c>
@@ -9255,7 +9280,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>9</v>
       </c>
@@ -9284,7 +9309,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>9</v>
       </c>
@@ -9313,7 +9338,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>9</v>
       </c>
@@ -9342,7 +9367,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>9</v>
       </c>
@@ -9371,7 +9396,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>9</v>
       </c>
@@ -9400,7 +9425,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="190" spans="1:9">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>9</v>
       </c>
@@ -9429,7 +9454,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>9</v>
       </c>
@@ -9458,7 +9483,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>9</v>
       </c>
@@ -9484,7 +9509,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>9</v>
       </c>
@@ -9513,7 +9538,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>9</v>
       </c>
@@ -9539,7 +9564,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="195" spans="1:9">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>9</v>
       </c>
@@ -9568,7 +9593,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="196" spans="1:9">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>9</v>
       </c>
@@ -9597,7 +9622,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>9</v>
       </c>
@@ -9623,7 +9648,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="198" spans="1:9">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>9</v>
       </c>
@@ -9652,7 +9677,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="199" spans="1:9">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>9</v>
       </c>
@@ -9678,7 +9703,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>9</v>
       </c>
@@ -9704,7 +9729,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>9</v>
       </c>
@@ -9730,7 +9755,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>9</v>
       </c>
@@ -9756,7 +9781,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>9</v>
       </c>
@@ -9785,7 +9810,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>9</v>
       </c>
@@ -9814,7 +9839,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>9</v>
       </c>
@@ -9843,7 +9868,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>9</v>
       </c>
@@ -9872,7 +9897,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="207" spans="1:9">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>9</v>
       </c>
@@ -9901,7 +9926,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="208" spans="1:9">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>9</v>
       </c>
@@ -9930,7 +9955,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="209" spans="1:9">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>9</v>
       </c>
@@ -9959,7 +9984,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="210" spans="1:9">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>9</v>
       </c>
@@ -9988,7 +10013,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="211" spans="1:9">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>9</v>
       </c>
@@ -10017,7 +10042,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="212" spans="1:9">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>9</v>
       </c>
@@ -10043,7 +10068,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="213" spans="1:9">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>9</v>
       </c>
@@ -10072,7 +10097,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="214" spans="1:9">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>9</v>
       </c>
@@ -10101,7 +10126,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="215" spans="1:9">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>9</v>
       </c>
@@ -10130,7 +10155,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>9</v>
       </c>
@@ -10159,7 +10184,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>9</v>
       </c>
@@ -10188,7 +10213,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="218" spans="1:9">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>9</v>
       </c>
@@ -10217,7 +10242,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>9</v>
       </c>
@@ -10246,7 +10271,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>9</v>
       </c>
@@ -10275,7 +10300,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>9</v>
       </c>
@@ -10301,7 +10326,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>9</v>
       </c>
@@ -10330,7 +10355,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>9</v>
       </c>
@@ -10359,7 +10384,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="224" spans="1:9">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>9</v>
       </c>
@@ -10388,7 +10413,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="225" spans="1:9">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>9</v>
       </c>
@@ -10417,7 +10442,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="226" spans="1:9">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>9</v>
       </c>
@@ -10446,7 +10471,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="227" spans="1:9">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>9</v>
       </c>
@@ -10475,7 +10500,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="228" spans="1:9">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>9</v>
       </c>
@@ -10504,7 +10529,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>9</v>
       </c>
@@ -10533,7 +10558,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="230" spans="1:9">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>9</v>
       </c>
@@ -10562,7 +10587,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="231" spans="1:9">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>9</v>
       </c>
@@ -10591,7 +10616,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>9</v>
       </c>
@@ -10620,7 +10645,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>9</v>
       </c>
@@ -10649,7 +10674,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="234" spans="1:9">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>9</v>
       </c>
@@ -10678,7 +10703,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="235" spans="1:9">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>9</v>
       </c>
@@ -10707,7 +10732,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="236" spans="1:9">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>9</v>
       </c>
@@ -10733,7 +10758,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="237" spans="1:9">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>9</v>
       </c>
@@ -10759,7 +10784,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="238" spans="1:9">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>9</v>
       </c>
@@ -10788,7 +10813,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="239" spans="1:9">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>9</v>
       </c>
@@ -10817,7 +10842,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="240" spans="1:9">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>9</v>
       </c>
@@ -10846,7 +10871,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="241" spans="1:9">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>9</v>
       </c>
@@ -10875,7 +10900,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="242" spans="1:9">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>9</v>
       </c>
@@ -10901,7 +10926,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="243" spans="1:9">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>9</v>
       </c>
@@ -10930,7 +10955,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="244" spans="1:9">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>9</v>
       </c>
@@ -10959,7 +10984,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="245" spans="1:9">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>9</v>
       </c>
@@ -10988,7 +11013,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="246" spans="1:9">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>9</v>
       </c>
@@ -11014,7 +11039,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="247" spans="1:9">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>9</v>
       </c>
@@ -11043,7 +11068,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>9</v>
       </c>
@@ -11072,7 +11097,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="249" spans="1:9">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>9</v>
       </c>
@@ -11101,7 +11126,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="250" spans="1:9">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>9</v>
       </c>
@@ -11130,7 +11155,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="251" spans="1:9">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>9</v>
       </c>
@@ -11159,7 +11184,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="252" spans="1:9">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>9</v>
       </c>
@@ -11185,7 +11210,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="253" spans="1:9">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>9</v>
       </c>
@@ -11211,7 +11236,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="254" spans="1:9">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>9</v>
       </c>
@@ -11240,7 +11265,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="255" spans="1:9">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>9</v>
       </c>
@@ -11269,7 +11294,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="256" spans="1:9">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>9</v>
       </c>
@@ -11298,7 +11323,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="257" spans="1:9">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>9</v>
       </c>
@@ -11327,7 +11352,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="258" spans="1:9">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>9</v>
       </c>
@@ -11356,7 +11381,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="259" spans="1:9">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>9</v>
       </c>
@@ -11385,7 +11410,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="260" spans="1:9">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>9</v>
       </c>
@@ -11411,7 +11436,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="261" spans="1:9">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>9</v>
       </c>
@@ -11440,7 +11465,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="262" spans="1:9">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>9</v>
       </c>
@@ -11469,7 +11494,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="263" spans="1:9">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>9</v>
       </c>
@@ -11498,7 +11523,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="264" spans="1:9">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>9</v>
       </c>
@@ -11527,7 +11552,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="265" spans="1:9">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>9</v>
       </c>
@@ -11556,7 +11581,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="266" spans="1:9">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>9</v>
       </c>
@@ -11585,7 +11610,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="267" spans="1:9">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>9</v>
       </c>
@@ -11611,7 +11636,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="268" spans="1:9">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>9</v>
       </c>
@@ -11640,7 +11665,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="269" spans="1:9">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>9</v>
       </c>
@@ -11669,7 +11694,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="270" spans="1:9">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>9</v>
       </c>
@@ -11698,7 +11723,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="271" spans="1:9">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>9</v>
       </c>
@@ -11724,7 +11749,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="272" spans="1:9">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>9</v>
       </c>
@@ -11753,7 +11778,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="273" spans="1:9">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>9</v>
       </c>
@@ -11782,7 +11807,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="274" spans="1:9">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>9</v>
       </c>
@@ -11811,7 +11836,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="275" spans="1:9">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>9</v>
       </c>
@@ -11840,7 +11865,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="276" spans="1:9">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>9</v>
       </c>
@@ -11866,7 +11891,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="277" spans="1:9">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>9</v>
       </c>
@@ -11892,7 +11917,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="278" spans="1:9">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>9</v>
       </c>
@@ -11915,7 +11940,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="279" spans="1:9">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>9</v>
       </c>
@@ -11938,7 +11963,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="280" spans="1:9">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>9</v>
       </c>
@@ -11964,7 +11989,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="281" spans="1:9">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>9</v>
       </c>

</xml_diff>